<commit_message>
made the tool more robust. Fixed stemming in documentsLoad. Fixed memory problem in java related to garbage collection.
</commit_message>
<xml_diff>
--- a/tool/sustainalize/longlist V2_small.xlsx
+++ b/tool/sustainalize/longlist V2_small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornr\source\repos\openmasses\tool\sustainalize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F1F953B3-CBC6-4958-BDCC-969B91B972A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2BF434BD-54F7-4D2A-A4CD-8CD7BD93AE40}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F10E0C21-3C48-4F4C-8325-1DE3E76C94DE}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>knowledge creation</t>
   </si>
   <si>
-    <t>Formation of new ideas</t>
-  </si>
-  <si>
     <t>sustainability research</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>new fancy knowledge creation</t>
+  </si>
+  <si>
+    <t>Formation of   new ideas</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:K944"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -584,10 +584,10 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -601,16 +601,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
       <c r="G4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -621,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
@@ -640,17 +640,17 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -661,15 +661,15 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>

</xml_diff>